<commit_message>
Updated step by step solution
</commit_message>
<xml_diff>
--- a/stackoverflow-survey-analysis/Stackoverflow Survey2020 Analysis Problem Solving.xlsx
+++ b/stackoverflow-survey-analysis/Stackoverflow Survey2020 Analysis Problem Solving.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t>Stackoverflow Developer Survey 2021 data analysis and prediction using Python</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Terbentuknya visualiasi pada varibel yg penting</t>
+  </si>
+  <si>
+    <t>Extract value (Pivot) EdLevel dengan Gender, plotkan</t>
+  </si>
+  <si>
+    <t>nested for loop, plt.barh()</t>
   </si>
   <si>
     <t>Menghitung jumlah responden berdasarkan jenjang pendidikan</t>
@@ -267,10 +273,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -303,24 +309,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,13 +333,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -349,8 +341,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -358,7 +364,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -381,6 +387,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -389,23 +409,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,6 +424,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,13 +438,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -448,187 +454,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,6 +776,54 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,45 +843,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -839,15 +854,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,152 +882,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1077,9 +1083,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -1407,10 +1410,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:H53"/>
+  <dimension ref="B2:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1530,7 +1533,7 @@
       <c r="F9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -1541,7 +1544,7 @@
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="12" t="s">
@@ -1558,7 +1561,7 @@
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -1573,7 +1576,7 @@
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="12" t="s">
         <v>31</v>
       </c>
@@ -1586,7 +1589,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="12" t="s">
         <v>33</v>
       </c>
@@ -1599,7 +1602,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="12" t="s">
         <v>35</v>
       </c>
@@ -1612,7 +1615,7 @@
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="18" t="s">
@@ -1729,70 +1732,68 @@
       <c r="H22" s="11"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="16"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="9">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="9">
         <v>4</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F26" s="11" t="s">
         <v>66</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>67</v>
@@ -1807,9 +1808,11 @@
         <v>68</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="11"/>
+        <v>63</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="9"/>
@@ -1817,10 +1820,10 @@
       <c r="D28" s="10"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="H28" s="11"/>
     </row>
@@ -1868,49 +1871,51 @@
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="F32" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="H32" s="11"/>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="16"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="9">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="9">
         <v>5</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -1921,39 +1926,41 @@
       <c r="D36" s="10"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="16"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="9">
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="9">
         <v>6</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="9"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="11"/>
@@ -1971,33 +1978,33 @@
       <c r="H40" s="11"/>
     </row>
     <row r="41" spans="2:8">
-      <c r="B41" s="14"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H41" s="16"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="2:8">
-      <c r="B42" s="9">
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="9">
         <v>7</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="9"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="11"/>
@@ -2015,33 +2022,33 @@
       <c r="H44" s="11"/>
     </row>
     <row r="45" spans="2:8">
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H45" s="16"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="9">
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="9">
         <v>8</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-    </row>
-    <row r="47" spans="2:8">
-      <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="11"/>
@@ -2059,33 +2066,33 @@
       <c r="H48" s="11"/>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="14"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" s="16"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
     </row>
     <row r="50" spans="2:8">
-      <c r="B50" s="9">
+      <c r="B50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="9">
         <v>9</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="9"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="11"/>
@@ -2103,49 +2110,58 @@
       <c r="H52" s="11"/>
     </row>
     <row r="53" spans="2:8">
-      <c r="B53" s="14"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H53" s="16"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="27">
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B24:B33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B16:B24"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B54"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="C9:C15"/>
-    <mergeCell ref="C16:C23"/>
-    <mergeCell ref="C24:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C16:C24"/>
+    <mergeCell ref="C25:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="C51:C54"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="D9:D15"/>
-    <mergeCell ref="D16:D23"/>
-    <mergeCell ref="D24:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="D16:D24"/>
+    <mergeCell ref="D25:D34"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D51:D54"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>